<commit_message>
adicion de los resultados de mondrian
</commit_message>
<xml_diff>
--- a/src/LSPM_LSPMW/resultados_ecrps.xlsx
+++ b/src/LSPM_LSPMW/resultados_ecrps.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G121"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,15 +456,10 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>LSPM_Hybrid</t>
+          <t>AREPD</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>AR_CPS</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>DeepAR</t>
         </is>
@@ -486,12 +481,9 @@
         <v>0.9937377995069321</v>
       </c>
       <c r="E2" t="n">
-        <v>1.045547991254877</v>
+        <v>0.4973774908684125</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4894490610586787</v>
-      </c>
-      <c r="G2" t="n">
         <v>0.7882456567571698</v>
       </c>
     </row>
@@ -511,12 +503,9 @@
         <v>1.571237421722828</v>
       </c>
       <c r="E3" t="n">
-        <v>1.653156527689611</v>
+        <v>0.7864228642675978</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7738869160485415</v>
-      </c>
-      <c r="G3" t="n">
         <v>1.246325714994318</v>
       </c>
     </row>
@@ -536,12 +525,9 @@
         <v>2.222065271508558</v>
       </c>
       <c r="E4" t="n">
-        <v>2.337916382184261</v>
+        <v>1.112169880582662</v>
       </c>
       <c r="F4" t="n">
-        <v>1.094441372604551</v>
-      </c>
-      <c r="G4" t="n">
         <v>1.762570773809471</v>
       </c>
     </row>
@@ -561,12 +547,9 @@
         <v>3.848729947987155</v>
       </c>
       <c r="E5" t="n">
-        <v>4.049389957790756</v>
+        <v>1.926334740126493</v>
       </c>
       <c r="F5" t="n">
-        <v>1.895628063584546</v>
-      </c>
-      <c r="G5" t="n">
         <v>3.052862185885275</v>
       </c>
     </row>
@@ -586,12 +569,9 @@
         <v>0.7237424763273413</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7411841810986272</v>
+        <v>0.6916182391405777</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7007101080773578</v>
-      </c>
-      <c r="G6" t="n">
         <v>0.7172476380798403</v>
       </c>
     </row>
@@ -611,12 +591,9 @@
         <v>1.081982503604247</v>
       </c>
       <c r="E7" t="n">
-        <v>1.099003687117958</v>
+        <v>0.9799148547462581</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9873448253744395</v>
-      </c>
-      <c r="G7" t="n">
         <v>1.15947180935163</v>
       </c>
     </row>
@@ -636,12 +613,9 @@
         <v>1.506994386246713</v>
       </c>
       <c r="E8" t="n">
-        <v>1.544902896953736</v>
+        <v>1.278127908543792</v>
       </c>
       <c r="F8" t="n">
-        <v>1.288830592747293</v>
-      </c>
-      <c r="G8" t="n">
         <v>1.627817182899139</v>
       </c>
     </row>
@@ -661,12 +635,9 @@
         <v>2.599971379483013</v>
       </c>
       <c r="E9" t="n">
-        <v>2.676219892198263</v>
+        <v>2.022300684581218</v>
       </c>
       <c r="F9" t="n">
-        <v>2.033550406272292</v>
-      </c>
-      <c r="G9" t="n">
         <v>2.774048941448051</v>
       </c>
     </row>
@@ -686,12 +657,9 @@
         <v>0.7259900670576133</v>
       </c>
       <c r="E10" t="n">
-        <v>0.759934648735814</v>
+        <v>0.4667584935757207</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4681271177883017</v>
-      </c>
-      <c r="G10" t="n">
         <v>0.9602135612672348</v>
       </c>
     </row>
@@ -711,12 +679,9 @@
         <v>1.147891085280217</v>
       </c>
       <c r="E11" t="n">
-        <v>1.201562181442585</v>
+        <v>0.7380099790751422</v>
       </c>
       <c r="F11" t="n">
-        <v>0.7401739638818974</v>
-      </c>
-      <c r="G11" t="n">
         <v>1.518213134424181</v>
       </c>
     </row>
@@ -736,12 +701,9 @@
         <v>1.623363140930455</v>
       </c>
       <c r="E12" t="n">
-        <v>1.699265533030705</v>
+        <v>1.043703722010225</v>
       </c>
       <c r="F12" t="n">
-        <v>1.046764058616007</v>
-      </c>
-      <c r="G12" t="n">
         <v>2.147089608328533</v>
       </c>
     </row>
@@ -761,12 +723,9 @@
         <v>2.811747439226143</v>
       </c>
       <c r="E13" t="n">
-        <v>2.943214238759791</v>
+        <v>1.807747875340081</v>
       </c>
       <c r="F13" t="n">
-        <v>1.81304853372935</v>
-      </c>
-      <c r="G13" t="n">
         <v>3.718884955144794</v>
       </c>
     </row>
@@ -786,12 +745,9 @@
         <v>0.5540869829588281</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5697508523723969</v>
+        <v>0.5238298342607568</v>
       </c>
       <c r="F14" t="n">
-        <v>0.5236122522501766</v>
-      </c>
-      <c r="G14" t="n">
         <v>0.611968748830326</v>
       </c>
     </row>
@@ -811,12 +767,9 @@
         <v>0.8215249470354513</v>
       </c>
       <c r="E15" t="n">
-        <v>0.8609938226805312</v>
+        <v>0.7492490298491818</v>
       </c>
       <c r="F15" t="n">
-        <v>0.7490605523573198</v>
-      </c>
-      <c r="G15" t="n">
         <v>0.9199134420647886</v>
       </c>
     </row>
@@ -836,12 +789,9 @@
         <v>1.161811721925374</v>
       </c>
       <c r="E16" t="n">
-        <v>1.217629141154263</v>
+        <v>1.05959814003477</v>
       </c>
       <c r="F16" t="n">
-        <v>1.059331592612772</v>
-      </c>
-      <c r="G16" t="n">
         <v>1.300954069674471</v>
       </c>
     </row>
@@ -861,12 +811,9 @@
         <v>2.012316931203831</v>
       </c>
       <c r="E17" t="n">
-        <v>2.108995537255639</v>
+        <v>1.835277814900657</v>
       </c>
       <c r="F17" t="n">
-        <v>1.834816141228778</v>
-      </c>
-      <c r="G17" t="n">
         <v>2.253318545877192</v>
       </c>
     </row>
@@ -886,12 +833,9 @@
         <v>1.519415365457544</v>
       </c>
       <c r="E18" t="n">
-        <v>1.594338032378002</v>
+        <v>0.5320928682482088</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5164441525307455</v>
-      </c>
-      <c r="G18" t="n">
         <v>1.666094785066689</v>
       </c>
     </row>
@@ -911,12 +855,9 @@
         <v>2.402406633351482</v>
       </c>
       <c r="E19" t="n">
-        <v>2.520869771272883</v>
+        <v>0.8413126952489799</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8165699031534047</v>
-      </c>
-      <c r="G19" t="n">
         <v>2.634331417815368</v>
       </c>
     </row>
@@ -936,12 +877,9 @@
         <v>3.397516043220755</v>
       </c>
       <c r="E20" t="n">
-        <v>3.565048219510473</v>
+        <v>1.189795823854022</v>
       </c>
       <c r="F20" t="n">
-        <v>1.15480423167743</v>
-      </c>
-      <c r="G20" t="n">
         <v>3.725511585324214</v>
       </c>
     </row>
@@ -961,12 +899,9 @@
         <v>5.884670406388724</v>
       </c>
       <c r="E21" t="n">
-        <v>6.174844647625104</v>
+        <v>2.060786817612509</v>
       </c>
       <c r="F21" t="n">
-        <v>2.000179602082413</v>
-      </c>
-      <c r="G21" t="n">
         <v>6.452764446991235</v>
       </c>
     </row>
@@ -986,12 +921,9 @@
         <v>0.256356225911444</v>
       </c>
       <c r="E22" t="n">
-        <v>0.259137001803698</v>
+        <v>0.2463713757894501</v>
       </c>
       <c r="F22" t="n">
-        <v>0.2460124272098335</v>
-      </c>
-      <c r="G22" t="n">
         <v>0.2528486530166831</v>
       </c>
     </row>
@@ -1011,12 +943,9 @@
         <v>0.4053347831224188</v>
       </c>
       <c r="E23" t="n">
-        <v>0.4097315758634235</v>
+        <v>0.3895473492986962</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3889798017641193</v>
-      </c>
-      <c r="G23" t="n">
         <v>0.3982018236251502</v>
       </c>
     </row>
@@ -1036,12 +965,9 @@
         <v>0.5732299475932816</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5794479515185542</v>
+        <v>0.5509031448617367</v>
       </c>
       <c r="F24" t="n">
-        <v>0.5501005114429415</v>
-      </c>
-      <c r="G24" t="n">
         <v>0.5632240479883953</v>
       </c>
     </row>
@@ -1061,12 +987,9 @@
         <v>0.9928633936516086</v>
       </c>
       <c r="E25" t="n">
-        <v>1.003633292371843</v>
+        <v>0.9541922374749561</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9528020356170991</v>
-      </c>
-      <c r="G25" t="n">
         <v>0.9793711075851492</v>
       </c>
     </row>
@@ -1086,12 +1009,9 @@
         <v>0.3725480064032503</v>
       </c>
       <c r="E26" t="n">
-        <v>0.3956774824141441</v>
+        <v>0.2775030480495396</v>
       </c>
       <c r="F26" t="n">
-        <v>0.2750236138489565</v>
-      </c>
-      <c r="G26" t="n">
         <v>0.2861676442085271</v>
       </c>
     </row>
@@ -1111,12 +1031,9 @@
         <v>0.4709601121091685</v>
       </c>
       <c r="E27" t="n">
-        <v>0.489128742218961</v>
+        <v>0.4582888732141183</v>
       </c>
       <c r="F27" t="n">
-        <v>0.4606976456744436</v>
-      </c>
-      <c r="G27" t="n">
         <v>0.4614289216785264</v>
       </c>
     </row>
@@ -1136,12 +1053,9 @@
         <v>0.6394364619536548</v>
       </c>
       <c r="E28" t="n">
-        <v>0.6488821588161927</v>
+        <v>0.6027756679145306</v>
       </c>
       <c r="F28" t="n">
-        <v>0.6060133163543698</v>
-      </c>
-      <c r="G28" t="n">
         <v>0.6462408787481445</v>
       </c>
     </row>
@@ -1161,12 +1075,9 @@
         <v>1.072120758094493</v>
       </c>
       <c r="E29" t="n">
-        <v>1.082099667799137</v>
+        <v>1.102237546908177</v>
       </c>
       <c r="F29" t="n">
-        <v>1.100793474813912</v>
-      </c>
-      <c r="G29" t="n">
         <v>1.087633819501489</v>
       </c>
     </row>
@@ -1186,12 +1097,9 @@
         <v>0.4751634545605972</v>
       </c>
       <c r="E30" t="n">
-        <v>0.4958170462384293</v>
+        <v>0.293562553705671</v>
       </c>
       <c r="F30" t="n">
-        <v>0.2986897415974247</v>
-      </c>
-      <c r="G30" t="n">
         <v>0.3858279060807383</v>
       </c>
     </row>
@@ -1211,12 +1119,9 @@
         <v>0.7512993886427047</v>
       </c>
       <c r="E31" t="n">
-        <v>0.7839555844252286</v>
+        <v>0.4641631529512067</v>
       </c>
       <c r="F31" t="n">
-        <v>0.4722699488130617</v>
-      </c>
-      <c r="G31" t="n">
         <v>0.6100434942575816</v>
       </c>
     </row>
@@ -1236,12 +1141,9 @@
         <v>1.062497784821128</v>
       </c>
       <c r="E32" t="n">
-        <v>1.108680619792284</v>
+        <v>0.6564258262203161</v>
       </c>
       <c r="F32" t="n">
-        <v>0.6678905668734499</v>
-      </c>
-      <c r="G32" t="n">
         <v>0.8627314154055642</v>
       </c>
     </row>
@@ -1261,12 +1163,9 @@
         <v>1.840300146239578</v>
       </c>
       <c r="E33" t="n">
-        <v>1.92029116284719</v>
+        <v>1.136962882701797</v>
       </c>
       <c r="F33" t="n">
-        <v>1.156820396004929</v>
-      </c>
-      <c r="G33" t="n">
         <v>1.4942994766705</v>
       </c>
     </row>
@@ -1286,12 +1185,9 @@
         <v>0.3049882053651976</v>
       </c>
       <c r="E34" t="n">
-        <v>0.3086096076441722</v>
+        <v>0.2943297381548295</v>
       </c>
       <c r="F34" t="n">
-        <v>0.294137366313069</v>
-      </c>
-      <c r="G34" t="n">
         <v>0.330134023987614</v>
       </c>
     </row>
@@ -1311,12 +1207,9 @@
         <v>0.4809378396881294</v>
       </c>
       <c r="E35" t="n">
-        <v>0.4873670910929975</v>
+        <v>0.4873269255781285</v>
       </c>
       <c r="F35" t="n">
-        <v>0.4871438182916745</v>
-      </c>
-      <c r="G35" t="n">
         <v>0.493632461181243</v>
       </c>
     </row>
@@ -1336,12 +1229,9 @@
         <v>0.6801488155453701</v>
       </c>
       <c r="E36" t="n">
-        <v>0.6892411500780409</v>
+        <v>0.6891843479139476</v>
       </c>
       <c r="F36" t="n">
-        <v>0.6889253951091987</v>
-      </c>
-      <c r="G36" t="n">
         <v>0.6980908897214296</v>
       </c>
     </row>
@@ -1361,12 +1251,9 @@
         <v>1.178052305232373</v>
       </c>
       <c r="E37" t="n">
-        <v>1.193800690602372</v>
+        <v>1.193702307166616</v>
       </c>
       <c r="F37" t="n">
-        <v>1.193253787757549</v>
-      </c>
-      <c r="G37" t="n">
         <v>1.209131552947393</v>
       </c>
     </row>
@@ -1386,12 +1273,9 @@
         <v>0.3013881402355498</v>
       </c>
       <c r="E38" t="n">
-        <v>0.304319535657165</v>
+        <v>0.2682972460351543</v>
       </c>
       <c r="F38" t="n">
-        <v>0.2716382351343758</v>
-      </c>
-      <c r="G38" t="n">
         <v>0.3380037476522882</v>
       </c>
     </row>
@@ -1411,12 +1295,9 @@
         <v>0.4765364914532871</v>
       </c>
       <c r="E39" t="n">
-        <v>0.481171434580734</v>
+        <v>0.4242151937501369</v>
       </c>
       <c r="F39" t="n">
-        <v>0.4294977613323092</v>
-      </c>
-      <c r="G39" t="n">
         <v>0.5344327958971102</v>
       </c>
     </row>
@@ -1436,12 +1317,9 @@
         <v>0.6739243691789291</v>
       </c>
       <c r="E40" t="n">
-        <v>0.6804791686105922</v>
+        <v>0.5999308803941873</v>
       </c>
       <c r="F40" t="n">
-        <v>0.6074015591034292</v>
-      </c>
-      <c r="G40" t="n">
         <v>0.7557909287584277</v>
       </c>
     </row>
@@ -1461,12 +1339,9 @@
         <v>1.16727124787671</v>
       </c>
       <c r="E41" t="n">
-        <v>1.178624493525774</v>
+        <v>1.039110765921769</v>
       </c>
       <c r="F41" t="n">
-        <v>1.0520503609962</v>
-      </c>
-      <c r="G41" t="n">
         <v>1.309023234555173</v>
       </c>
     </row>
@@ -1486,12 +1361,9 @@
         <v>0.4230251640456619</v>
       </c>
       <c r="E42" t="n">
-        <v>0.4423648133870445</v>
+        <v>0.333349992110206</v>
       </c>
       <c r="F42" t="n">
-        <v>0.3292812180733002</v>
-      </c>
-      <c r="G42" t="n">
         <v>0.4098535085051987</v>
       </c>
     </row>
@@ -1511,12 +1383,9 @@
         <v>0.6688615129753304</v>
       </c>
       <c r="E43" t="n">
-        <v>0.6994401835092026</v>
+        <v>0.5270726184830601</v>
       </c>
       <c r="F43" t="n">
-        <v>0.5206393218224219</v>
-      </c>
-      <c r="G43" t="n">
         <v>0.6480347590509137</v>
       </c>
     </row>
@@ -1536,12 +1405,9 @@
         <v>0.9459130229990996</v>
       </c>
       <c r="E44" t="n">
-        <v>0.9891577935874405</v>
+        <v>0.7453932468036716</v>
       </c>
       <c r="F44" t="n">
-        <v>0.7362951913868826</v>
-      </c>
-      <c r="G44" t="n">
         <v>0.9164596051944787</v>
       </c>
     </row>
@@ -1561,12 +1427,9 @@
         <v>1.638369415375509</v>
       </c>
       <c r="E45" t="n">
-        <v>1.713271555196175</v>
+        <v>1.291058977538255</v>
       </c>
       <c r="F45" t="n">
-        <v>1.275300683255852</v>
-      </c>
-      <c r="G45" t="n">
         <v>1.58735464944723</v>
       </c>
     </row>
@@ -1586,12 +1449,9 @@
         <v>0.425179511647227</v>
       </c>
       <c r="E46" t="n">
-        <v>0.4327940712252755</v>
+        <v>0.3831618596250905</v>
       </c>
       <c r="F46" t="n">
-        <v>0.3874028695705691</v>
-      </c>
-      <c r="G46" t="n">
         <v>0.421875779305018</v>
       </c>
     </row>
@@ -1611,12 +1471,9 @@
         <v>0.6272325064280376</v>
       </c>
       <c r="E47" t="n">
-        <v>0.6396288023335612</v>
+        <v>0.5713886282109188</v>
       </c>
       <c r="F47" t="n">
-        <v>0.5721558616602909</v>
-      </c>
-      <c r="G47" t="n">
         <v>0.777072896129946</v>
       </c>
     </row>
@@ -1636,12 +1493,9 @@
         <v>0.8982211850840237</v>
       </c>
       <c r="E48" t="n">
-        <v>0.9242865888676881</v>
+        <v>0.8337172116731276</v>
       </c>
       <c r="F48" t="n">
-        <v>0.8433054478670613</v>
-      </c>
-      <c r="G48" t="n">
         <v>0.9950470076988573</v>
       </c>
     </row>
@@ -1661,12 +1515,9 @@
         <v>1.587791026368035</v>
       </c>
       <c r="E49" t="n">
-        <v>1.644048504494153</v>
+        <v>1.389374859862545</v>
       </c>
       <c r="F49" t="n">
-        <v>1.403576935656104</v>
-      </c>
-      <c r="G49" t="n">
         <v>1.864640989415002</v>
       </c>
     </row>
@@ -1686,12 +1537,9 @@
         <v>0.5576467794808115</v>
       </c>
       <c r="E50" t="n">
-        <v>0.586749750344595</v>
+        <v>0.3670943026531545</v>
       </c>
       <c r="F50" t="n">
-        <v>0.3692261386450841</v>
-      </c>
-      <c r="G50" t="n">
         <v>0.7398078656037065</v>
       </c>
     </row>
@@ -1711,12 +1559,9 @@
         <v>0.8817169765085061</v>
       </c>
       <c r="E51" t="n">
-        <v>0.9277328138120432</v>
+        <v>0.5804270566047248</v>
       </c>
       <c r="F51" t="n">
-        <v>0.5837977852478932</v>
-      </c>
-      <c r="G51" t="n">
         <v>1.169739166947383</v>
       </c>
     </row>
@@ -1736,12 +1581,9 @@
         <v>1.24693610635293</v>
       </c>
       <c r="E52" t="n">
-        <v>1.312012327551545</v>
+        <v>0.820847815687512</v>
       </c>
       <c r="F52" t="n">
-        <v>0.8256147458333364</v>
-      </c>
-      <c r="G52" t="n">
         <v>1.654262714764873</v>
       </c>
     </row>
@@ -1761,12 +1603,9 @@
         <v>2.159756689995384</v>
       </c>
       <c r="E53" t="n">
-        <v>2.272472011475977</v>
+        <v>1.421750122527787</v>
       </c>
       <c r="F53" t="n">
-        <v>1.43000668770746</v>
-      </c>
-      <c r="G53" t="n">
         <v>2.865261842932972</v>
       </c>
     </row>
@@ -1786,12 +1625,9 @@
         <v>0.3825845137620879</v>
       </c>
       <c r="E54" t="n">
-        <v>0.3937846473592227</v>
+        <v>0.3882721366937972</v>
       </c>
       <c r="F54" t="n">
-        <v>0.3880812997879651</v>
-      </c>
-      <c r="G54" t="n">
         <v>0.3874581232386796</v>
       </c>
     </row>
@@ -1811,12 +1647,9 @@
         <v>0.571639807529026</v>
       </c>
       <c r="E55" t="n">
-        <v>0.6083794737997821</v>
+        <v>0.5712798286408199</v>
       </c>
       <c r="F55" t="n">
-        <v>0.5708836552528523</v>
-      </c>
-      <c r="G55" t="n">
         <v>0.5964606202209258</v>
       </c>
     </row>
@@ -1836,12 +1669,9 @@
         <v>0.8084207685998944</v>
       </c>
       <c r="E56" t="n">
-        <v>0.860378502917059</v>
+        <v>0.8079116816806418</v>
       </c>
       <c r="F56" t="n">
-        <v>0.807351407907842</v>
-      </c>
-      <c r="G56" t="n">
         <v>0.8435228172325123</v>
       </c>
     </row>
@@ -1861,12 +1691,9 @@
         <v>1.400225845108899</v>
       </c>
       <c r="E57" t="n">
-        <v>1.490219280792394</v>
+        <v>1.399344080887712</v>
       </c>
       <c r="F57" t="n">
-        <v>1.398373658256821</v>
-      </c>
-      <c r="G57" t="n">
         <v>1.461024323317255</v>
       </c>
     </row>
@@ -1886,12 +1713,9 @@
         <v>0.6457280842841988</v>
       </c>
       <c r="E58" t="n">
-        <v>0.6992653675540016</v>
+        <v>0.3566436544245287</v>
       </c>
       <c r="F58" t="n">
-        <v>0.3585419596271048</v>
-      </c>
-      <c r="G58" t="n">
         <v>0.4309220338374184</v>
       </c>
     </row>
@@ -1911,12 +1735,9 @@
         <v>1.020985747737623</v>
       </c>
       <c r="E59" t="n">
-        <v>1.105635625172725</v>
+        <v>0.56390313084634</v>
       </c>
       <c r="F59" t="n">
-        <v>0.566904614904191</v>
-      </c>
-      <c r="G59" t="n">
         <v>0.6813488208604352</v>
       </c>
     </row>
@@ -1936,12 +1757,9 @@
         <v>1.443891891440182</v>
       </c>
       <c r="E60" t="n">
-        <v>1.563604896162123</v>
+        <v>0.7974794557446048</v>
       </c>
       <c r="F60" t="n">
-        <v>0.8017241951998406</v>
-      </c>
-      <c r="G60" t="n">
         <v>0.9635735293463937</v>
       </c>
     </row>
@@ -1961,12 +1779,9 @@
         <v>2.500894116611121</v>
       </c>
       <c r="E61" t="n">
-        <v>2.708243123116255</v>
+        <v>1.381274935760989</v>
       </c>
       <c r="F61" t="n">
-        <v>1.388627040150644</v>
-      </c>
-      <c r="G61" t="n">
         <v>1.668954905379568</v>
       </c>
     </row>
@@ -1986,12 +1801,9 @@
         <v>0.3388872701420261</v>
       </c>
       <c r="E62" t="n">
-        <v>0.3466337418367348</v>
+        <v>0.3261172872926709</v>
       </c>
       <c r="F62" t="n">
-        <v>0.3193260396337934</v>
-      </c>
-      <c r="G62" t="n">
         <v>0.3692678394818738</v>
       </c>
     </row>
@@ -2011,12 +1823,9 @@
         <v>0.5358278218427879</v>
       </c>
       <c r="E63" t="n">
-        <v>0.5480760690354398</v>
+        <v>0.5156367073967559</v>
       </c>
       <c r="F63" t="n">
-        <v>0.5048988018899524</v>
-      </c>
-      <c r="G63" t="n">
         <v>0.5838636940289806</v>
       </c>
     </row>
@@ -2036,12 +1845,9 @@
         <v>0.757774972746905</v>
       </c>
       <c r="E64" t="n">
-        <v>0.7750966100420514</v>
+        <v>0.7292204257820608</v>
       </c>
       <c r="F64" t="n">
-        <v>0.714034734091173</v>
-      </c>
-      <c r="G64" t="n">
         <v>0.8257080014454607</v>
       </c>
     </row>
@@ -2061,12 +1867,9 @@
         <v>1.312504753501761</v>
       </c>
       <c r="E65" t="n">
-        <v>1.342506709367234</v>
+        <v>1.263046829004834</v>
       </c>
       <c r="F65" t="n">
-        <v>1.236744439286102</v>
-      </c>
-      <c r="G65" t="n">
         <v>1.430168182416155</v>
       </c>
     </row>
@@ -2086,12 +1889,9 @@
         <v>0.4749860643750106</v>
       </c>
       <c r="E66" t="n">
-        <v>0.5004435140335642</v>
+        <v>0.323363459970064</v>
       </c>
       <c r="F66" t="n">
-        <v>0.3240844917197842</v>
-      </c>
-      <c r="G66" t="n">
         <v>0.3791988086149213</v>
       </c>
     </row>
@@ -2111,12 +1911,9 @@
         <v>0.5694205744214005</v>
       </c>
       <c r="E67" t="n">
-        <v>0.5729162534529303</v>
+        <v>0.5261384191813171</v>
       </c>
       <c r="F67" t="n">
-        <v>0.5271793286483137</v>
-      </c>
-      <c r="G67" t="n">
         <v>0.592742517913008</v>
       </c>
     </row>
@@ -2136,12 +1933,9 @@
         <v>0.7758833746224847</v>
       </c>
       <c r="E68" t="n">
-        <v>0.7929622604649376</v>
+        <v>0.7993812799942137</v>
       </c>
       <c r="F68" t="n">
-        <v>0.8100146702107459</v>
-      </c>
-      <c r="G68" t="n">
         <v>1.019387987809437</v>
       </c>
     </row>
@@ -2161,12 +1955,9 @@
         <v>1.39987758123136</v>
       </c>
       <c r="E69" t="n">
-        <v>1.440690321066953</v>
+        <v>1.355419243126418</v>
       </c>
       <c r="F69" t="n">
-        <v>1.357231263815395</v>
-      </c>
-      <c r="G69" t="n">
         <v>1.660406605501418</v>
       </c>
     </row>
@@ -2186,12 +1977,9 @@
         <v>0.7173279686819941</v>
       </c>
       <c r="E70" t="n">
-        <v>0.7438571378346043</v>
+        <v>0.3597941337315489</v>
       </c>
       <c r="F70" t="n">
-        <v>0.3623649498824421</v>
-      </c>
-      <c r="G70" t="n">
         <v>0.7815090274682025</v>
       </c>
     </row>
@@ -2211,12 +1999,9 @@
         <v>1.134195105188516</v>
       </c>
       <c r="E71" t="n">
-        <v>1.17614140466558</v>
+        <v>0.5688844757741804</v>
       </c>
       <c r="F71" t="n">
-        <v>0.5729492929987541</v>
-      </c>
-      <c r="G71" t="n">
         <v>1.235674189548996</v>
       </c>
     </row>
@@ -2236,12 +2021,9 @@
         <v>1.603994100134778</v>
       </c>
       <c r="E72" t="n">
-        <v>1.663315125746605</v>
+        <v>0.8045241411308707</v>
       </c>
       <c r="F72" t="n">
-        <v>0.8102726607665904</v>
-      </c>
-      <c r="G72" t="n">
         <v>1.747507624100864</v>
       </c>
     </row>
@@ -2261,12 +2043,9 @@
         <v>2.778199276474157</v>
       </c>
       <c r="E73" t="n">
-        <v>2.880946306790936</v>
+        <v>1.393476688473705</v>
       </c>
       <c r="F73" t="n">
-        <v>1.403433416530154</v>
-      </c>
-      <c r="G73" t="n">
         <v>3.026771269376774</v>
       </c>
     </row>
@@ -2286,12 +2065,9 @@
         <v>0.3632042989810351</v>
       </c>
       <c r="E74" t="n">
-        <v>0.371742697003576</v>
+        <v>0.3663325988101349</v>
       </c>
       <c r="F74" t="n">
-        <v>0.3671180334164296</v>
-      </c>
-      <c r="G74" t="n">
         <v>0.3749897835769944</v>
       </c>
     </row>
@@ -2311,12 +2087,9 @@
         <v>0.5748088053769973</v>
       </c>
       <c r="E75" t="n">
-        <v>0.5888116463475366</v>
+        <v>0.5742030603060621</v>
       </c>
       <c r="F75" t="n">
-        <v>0.5738840437461679</v>
-      </c>
-      <c r="G75" t="n">
         <v>0.6138524535031745</v>
       </c>
     </row>
@@ -2336,12 +2109,9 @@
         <v>0.8129024083356264</v>
       </c>
       <c r="E76" t="n">
-        <v>0.8327054159479167</v>
+        <v>0.8120457559062384</v>
       </c>
       <c r="F76" t="n">
-        <v>0.8115945983646951</v>
-      </c>
-      <c r="G76" t="n">
         <v>0.868118623043702</v>
       </c>
     </row>
@@ -2361,12 +2131,9 @@
         <v>1.407988272832407</v>
       </c>
       <c r="E77" t="n">
-        <v>1.442288088159567</v>
+        <v>1.406504508122562</v>
       </c>
       <c r="F77" t="n">
-        <v>1.405723080345603</v>
-      </c>
-      <c r="G77" t="n">
         <v>1.503625712689522</v>
       </c>
     </row>
@@ -2386,12 +2153,9 @@
         <v>0.3632788417737464</v>
       </c>
       <c r="E78" t="n">
-        <v>0.3637199226839637</v>
+        <v>0.3676647461812403</v>
       </c>
       <c r="F78" t="n">
-        <v>0.3658748967072356</v>
-      </c>
-      <c r="G78" t="n">
         <v>0.4967403078593161</v>
       </c>
     </row>
@@ -2411,12 +2175,9 @@
         <v>0.574394282876481</v>
       </c>
       <c r="E79" t="n">
-        <v>0.5750916930308344</v>
+        <v>0.581329006843032</v>
       </c>
       <c r="F79" t="n">
-        <v>0.5784990063254168</v>
-      </c>
-      <c r="G79" t="n">
         <v>0.7854159896535239</v>
       </c>
     </row>
@@ -2436,12 +2197,9 @@
         <v>0.8123161849934872</v>
       </c>
       <c r="E80" t="n">
-        <v>0.8133024718923106</v>
+        <v>0.8221233658228639</v>
       </c>
       <c r="F80" t="n">
-        <v>0.8181211406991652</v>
-      </c>
-      <c r="G80" t="n">
         <v>1.110745490713039</v>
       </c>
     </row>
@@ -2461,12 +2219,9 @@
         <v>1.406972904219239</v>
       </c>
       <c r="E81" t="n">
-        <v>1.408681203238841</v>
+        <v>1.42395943995023</v>
       </c>
       <c r="F81" t="n">
-        <v>1.417027382674692</v>
-      </c>
-      <c r="G81" t="n">
         <v>1.923868901996728</v>
       </c>
     </row>
@@ -2486,12 +2241,9 @@
         <v>0.2889511445810004</v>
       </c>
       <c r="E82" t="n">
-        <v>0.2918664392691306</v>
+        <v>0.2938265160403427</v>
       </c>
       <c r="F82" t="n">
-        <v>0.2935195431847861</v>
-      </c>
-      <c r="G82" t="n">
         <v>0.3484782649751727</v>
       </c>
     </row>
@@ -2511,12 +2263,9 @@
         <v>0.4568718746942906</v>
       </c>
       <c r="E83" t="n">
-        <v>0.4614813603268315</v>
+        <v>0.46458051411673</v>
       </c>
       <c r="F83" t="n">
-        <v>0.4640951474111571</v>
-      </c>
-      <c r="G83" t="n">
         <v>0.550992736000266</v>
       </c>
     </row>
@@ -2536,12 +2285,9 @@
         <v>0.6461144014594867</v>
       </c>
       <c r="E84" t="n">
-        <v>0.6526331985565901</v>
+        <v>0.6570160640898277</v>
       </c>
       <c r="F84" t="n">
-        <v>0.6563296519093232</v>
-      </c>
-      <c r="G84" t="n">
         <v>0.7792212427067328</v>
       </c>
     </row>
@@ -2561,12 +2307,9 @@
         <v>1.119102970829786</v>
       </c>
       <c r="E85" t="n">
-        <v>1.130393858606201</v>
+        <v>1.137985204766624</v>
       </c>
       <c r="F85" t="n">
-        <v>1.136796303990181</v>
-      </c>
-      <c r="G85" t="n">
         <v>1.349650828435824</v>
       </c>
     </row>
@@ -2586,12 +2329,9 @@
         <v>0.3666713252616645</v>
       </c>
       <c r="E86" t="n">
-        <v>0.4091656223122435</v>
+        <v>0.2900111740867778</v>
       </c>
       <c r="F86" t="n">
-        <v>0.2893066579566861</v>
-      </c>
-      <c r="G86" t="n">
         <v>0.3227320349290743</v>
       </c>
     </row>
@@ -2611,12 +2351,9 @@
         <v>0.4794156191632496</v>
       </c>
       <c r="E87" t="n">
-        <v>0.4823907044326844</v>
+        <v>0.479860673596569</v>
       </c>
       <c r="F87" t="n">
-        <v>0.4834371446890975</v>
-      </c>
-      <c r="G87" t="n">
         <v>0.5315145456787626</v>
       </c>
     </row>
@@ -2636,12 +2373,9 @@
         <v>0.6516276902532168</v>
       </c>
       <c r="E88" t="n">
-        <v>0.6575176000741851</v>
+        <v>0.6958923643603879</v>
       </c>
       <c r="F88" t="n">
-        <v>0.703039891466038</v>
-      </c>
-      <c r="G88" t="n">
         <v>0.784068281369689</v>
       </c>
     </row>
@@ -2661,12 +2395,9 @@
         <v>1.139487149768482</v>
       </c>
       <c r="E89" t="n">
-        <v>1.160611325735809</v>
+        <v>1.009705981626627</v>
       </c>
       <c r="F89" t="n">
-        <v>1.014416094787409</v>
-      </c>
-      <c r="G89" t="n">
         <v>1.426237663513117</v>
       </c>
     </row>
@@ -2686,12 +2417,9 @@
         <v>0.5031173132679549</v>
       </c>
       <c r="E90" t="n">
-        <v>0.525689229866993</v>
+        <v>0.3212427504052819</v>
       </c>
       <c r="F90" t="n">
-        <v>0.3288594159580669</v>
-      </c>
-      <c r="G90" t="n">
         <v>0.4740160008058193</v>
       </c>
     </row>
@@ -2711,12 +2439,9 @@
         <v>0.7954983200955943</v>
       </c>
       <c r="E91" t="n">
-        <v>0.8311876538997554</v>
+        <v>0.5079293870327007</v>
       </c>
       <c r="F91" t="n">
-        <v>0.5199723926858779</v>
-      </c>
-      <c r="G91" t="n">
         <v>0.7494851924394931</v>
       </c>
     </row>
@@ -2736,12 +2461,9 @@
         <v>1.125004513124203</v>
       </c>
       <c r="E92" t="n">
-        <v>1.175476853022108</v>
+        <v>0.7231160712417757</v>
       </c>
       <c r="F92" t="n">
-        <v>0.7401748548604892</v>
-      </c>
-      <c r="G92" t="n">
         <v>1.059931866315031</v>
       </c>
     </row>
@@ -2761,12 +2483,9 @@
         <v>1.948564975475409</v>
       </c>
       <c r="E93" t="n">
-        <v>2.035985632555466</v>
+        <v>1.252473775644718</v>
       </c>
       <c r="F93" t="n">
-        <v>1.282020455583678</v>
-      </c>
-      <c r="G93" t="n">
         <v>1.835855624865762</v>
       </c>
     </row>
@@ -2786,12 +2505,9 @@
         <v>0.320964150259555</v>
       </c>
       <c r="E94" t="n">
-        <v>0.3264452494645119</v>
+        <v>0.3241796591354696</v>
       </c>
       <c r="F94" t="n">
-        <v>0.3248666859852042</v>
-      </c>
-      <c r="G94" t="n">
         <v>0.3212714040731273</v>
       </c>
     </row>
@@ -2811,12 +2527,9 @@
         <v>0.4975382720627743</v>
       </c>
       <c r="E95" t="n">
-        <v>0.505759412698517</v>
+        <v>0.4895632710469722</v>
       </c>
       <c r="F95" t="n">
-        <v>0.489136806619892</v>
-      </c>
-      <c r="G95" t="n">
         <v>0.5145678343063389</v>
       </c>
     </row>
@@ -2836,12 +2549,9 @@
         <v>0.7036253721508502</v>
       </c>
       <c r="E96" t="n">
-        <v>0.7152518207360941</v>
+        <v>0.6923470178120374</v>
       </c>
       <c r="F96" t="n">
-        <v>0.6917439060347966</v>
-      </c>
-      <c r="G96" t="n">
         <v>0.727708908105423</v>
       </c>
     </row>
@@ -2861,12 +2571,9 @@
         <v>1.218714894059832</v>
       </c>
       <c r="E97" t="n">
-        <v>1.238852493721061</v>
+        <v>1.199180211774637</v>
       </c>
       <c r="F97" t="n">
-        <v>1.198135591532763</v>
-      </c>
-      <c r="G97" t="n">
         <v>1.260428375676063</v>
       </c>
     </row>
@@ -2886,12 +2593,9 @@
         <v>0.3256580327720072</v>
       </c>
       <c r="E98" t="n">
-        <v>0.3256092456991056</v>
+        <v>0.2937951268051074</v>
       </c>
       <c r="F98" t="n">
-        <v>0.2983709033244978</v>
-      </c>
-      <c r="G98" t="n">
         <v>0.4651224200995622</v>
       </c>
     </row>
@@ -2911,12 +2615,9 @@
         <v>0.5149105609446504</v>
       </c>
       <c r="E99" t="n">
-        <v>0.5148334218092794</v>
+        <v>0.464530883153097</v>
       </c>
       <c r="F99" t="n">
-        <v>0.4717658210257434</v>
-      </c>
-      <c r="G99" t="n">
         <v>0.7354230262538396</v>
       </c>
     </row>
@@ -2936,12 +2637,9 @@
         <v>0.7281934986970625</v>
       </c>
       <c r="E100" t="n">
-        <v>0.7280844074856311</v>
+        <v>0.6569458751476042</v>
       </c>
       <c r="F100" t="n">
-        <v>0.6671776223672975</v>
-      </c>
-      <c r="G100" t="n">
         <v>1.040045246013243</v>
       </c>
     </row>
@@ -2961,12 +2659,9 @@
         <v>1.261268137484653</v>
       </c>
       <c r="E101" t="n">
-        <v>1.261079185963795</v>
+        <v>1.13786363366919</v>
       </c>
       <c r="F101" t="n">
-        <v>1.155585539628383</v>
-      </c>
-      <c r="G101" t="n">
         <v>1.801411131247476</v>
       </c>
     </row>
@@ -2986,12 +2681,9 @@
         <v>0.2567316840534696</v>
       </c>
       <c r="E102" t="n">
-        <v>0.2610666803346058</v>
+        <v>0.2302353110257249</v>
       </c>
       <c r="F102" t="n">
-        <v>0.23107723864347</v>
-      </c>
-      <c r="G102" t="n">
         <v>0.2619391610911026</v>
       </c>
     </row>
@@ -3011,12 +2703,9 @@
         <v>0.4059284345698468</v>
       </c>
       <c r="E103" t="n">
-        <v>0.4127826655182219</v>
+        <v>0.3640339921243255</v>
       </c>
       <c r="F103" t="n">
-        <v>0.3653651966012468</v>
-      </c>
-      <c r="G103" t="n">
         <v>0.4895743540340289</v>
       </c>
     </row>
@@ -3036,12 +2725,9 @@
         <v>0.5740694975215568</v>
       </c>
       <c r="E104" t="n">
-        <v>0.5837628438883864</v>
+        <v>0.5148218101136067</v>
       </c>
       <c r="F104" t="n">
-        <v>0.5167044175593918</v>
-      </c>
-      <c r="G104" t="n">
         <v>0.6031671170322137</v>
       </c>
     </row>
@@ -3061,12 +2747,9 @@
         <v>0.9943175367828719</v>
       </c>
       <c r="E105" t="n">
-        <v>1.011106905185584</v>
+        <v>0.8916975342351248</v>
       </c>
       <c r="F105" t="n">
-        <v>0.8949583060176874</v>
-      </c>
-      <c r="G105" t="n">
         <v>1.037983989766804</v>
       </c>
     </row>
@@ -3086,12 +2769,9 @@
         <v>0.2956325539783811</v>
       </c>
       <c r="E106" t="n">
-        <v>0.3050651451239353</v>
+        <v>0.2734755917489923</v>
       </c>
       <c r="F106" t="n">
-        <v>0.2737873405205885</v>
-      </c>
-      <c r="G106" t="n">
         <v>0.2840413399622524</v>
       </c>
     </row>
@@ -3111,12 +2791,9 @@
         <v>0.450463771290905</v>
       </c>
       <c r="E107" t="n">
-        <v>0.4493297127878835</v>
+        <v>0.4519030817654087</v>
       </c>
       <c r="F107" t="n">
-        <v>0.4523445327360684</v>
-      </c>
-      <c r="G107" t="n">
         <v>0.4539475731409468</v>
       </c>
     </row>
@@ -3136,12 +2813,9 @@
         <v>0.6155800440702258</v>
       </c>
       <c r="E108" t="n">
-        <v>0.6226214576213395</v>
+        <v>0.6243045595450443</v>
       </c>
       <c r="F108" t="n">
-        <v>0.6280918213970788</v>
-      </c>
-      <c r="G108" t="n">
         <v>0.6996074991788701</v>
       </c>
     </row>
@@ -3161,12 +2835,9 @@
         <v>1.053843768183732</v>
       </c>
       <c r="E109" t="n">
-        <v>1.071327336495102</v>
+        <v>1.005609033244776</v>
       </c>
       <c r="F109" t="n">
-        <v>1.011911558914227</v>
-      </c>
-      <c r="G109" t="n">
         <v>1.069577379412743</v>
       </c>
     </row>
@@ -3186,12 +2857,9 @@
         <v>0.4117544732276799</v>
       </c>
       <c r="E110" t="n">
-        <v>0.4318050657745773</v>
+        <v>0.2811468762106081</v>
       </c>
       <c r="F110" t="n">
-        <v>0.2848581339171007</v>
-      </c>
-      <c r="G110" t="n">
         <v>0.4617747839850514</v>
       </c>
     </row>
@@ -3211,12 +2879,9 @@
         <v>0.651040986081146</v>
       </c>
       <c r="E111" t="n">
-        <v>0.682743756523242</v>
+        <v>0.4445322432061768</v>
       </c>
       <c r="F111" t="n">
-        <v>0.4504002568784154</v>
-      </c>
-      <c r="G111" t="n">
         <v>0.7300528904188193</v>
       </c>
     </row>
@@ -3236,12 +2901,9 @@
         <v>0.9207109921767098</v>
       </c>
       <c r="E112" t="n">
-        <v>0.9655454801007231</v>
+        <v>0.6286635274486887</v>
       </c>
       <c r="F112" t="n">
-        <v>0.6369621519710486</v>
-      </c>
-      <c r="G112" t="n">
         <v>1.032565406427265</v>
       </c>
     </row>
@@ -3261,12 +2923,9 @@
         <v>1.594718217537212</v>
       </c>
       <c r="E113" t="n">
-        <v>1.672373828552936</v>
+        <v>1.08887717075013</v>
       </c>
       <c r="F113" t="n">
-        <v>1.103250810060901</v>
-      </c>
-      <c r="G113" t="n">
         <v>1.788381180203815</v>
       </c>
     </row>
@@ -3286,12 +2945,9 @@
         <v>0.288692807787654</v>
       </c>
       <c r="E114" t="n">
-        <v>0.2884529337275099</v>
+        <v>0.2934806427050045</v>
       </c>
       <c r="F114" t="n">
-        <v>0.294732216661629</v>
-      </c>
-      <c r="G114" t="n">
         <v>0.2877908775033957</v>
       </c>
     </row>
@@ -3311,12 +2967,9 @@
         <v>0.4389148255179283</v>
       </c>
       <c r="E115" t="n">
-        <v>0.4466140189539541</v>
+        <v>0.4367769228965578</v>
       </c>
       <c r="F115" t="n">
-        <v>0.4360678895977292</v>
-      </c>
-      <c r="G115" t="n">
         <v>0.4430852324024483</v>
       </c>
     </row>
@@ -3336,12 +2989,9 @@
         <v>0.620719298974075</v>
       </c>
       <c r="E116" t="n">
-        <v>0.6316076027506365</v>
+        <v>0.6176958482887239</v>
       </c>
       <c r="F116" t="n">
-        <v>0.6166931237784576</v>
-      </c>
-      <c r="G116" t="n">
         <v>0.6266176544538866</v>
       </c>
     </row>
@@ -3361,12 +3011,9 @@
         <v>1.075117363061634</v>
       </c>
       <c r="E117" t="n">
-        <v>1.093976458410882</v>
+        <v>1.06988059320828</v>
       </c>
       <c r="F117" t="n">
-        <v>1.068143823405399</v>
-      </c>
-      <c r="G117" t="n">
         <v>1.085333520944334</v>
       </c>
     </row>
@@ -3386,12 +3033,9 @@
         <v>0.2894112078274844</v>
       </c>
       <c r="E118" t="n">
-        <v>0.3018749286283951</v>
+        <v>0.2605439295569679</v>
       </c>
       <c r="F118" t="n">
-        <v>0.2606143178924125</v>
-      </c>
-      <c r="G118" t="n">
         <v>0.3112321980868709</v>
       </c>
     </row>
@@ -3411,12 +3055,9 @@
         <v>0.457599298557601</v>
       </c>
       <c r="E119" t="n">
-        <v>0.4773061714832489</v>
+        <v>0.4119561245473469</v>
       </c>
       <c r="F119" t="n">
-        <v>0.4120674184025341</v>
-      </c>
-      <c r="G119" t="n">
         <v>0.4921012984152725</v>
       </c>
     </row>
@@ -3436,12 +3077,9 @@
         <v>0.6471431341525743</v>
       </c>
       <c r="E120" t="n">
-        <v>0.6750128611159887</v>
+        <v>0.5825939388524203</v>
       </c>
       <c r="F120" t="n">
-        <v>0.5827513322208093</v>
-      </c>
-      <c r="G120" t="n">
         <v>0.6959363137855992</v>
       </c>
     </row>
@@ -3461,12 +3099,9 @@
         <v>1.12088478812162</v>
       </c>
       <c r="E121" t="n">
-        <v>1.169156571215327</v>
+        <v>1.009082303007336</v>
       </c>
       <c r="F121" t="n">
-        <v>1.009354916475408</v>
-      </c>
-      <c r="G121" t="n">
         <v>1.205397154650455</v>
       </c>
     </row>

</xml_diff>